<commit_message>
python translate files finish
</commit_message>
<xml_diff>
--- a/shop_sys_tool/shop_items_list.xlsx
+++ b/shop_sys_tool/shop_items_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>物品</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>ancientfruit_gem</t>
+  </si>
+  <si>
+    <t>噩梦花瓣</t>
+  </si>
+  <si>
+    <t>petals_evil</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1085,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1479,6 +1485,38 @@
         <v>15</v>
       </c>
       <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
shop item param is_permanent added
</commit_message>
<xml_diff>
--- a/shop_sys_tool/shop_items_list.xlsx
+++ b/shop_sys_tool/shop_items_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>物品</t>
   </si>
@@ -61,6 +61,9 @@
     <t>图片tex名字。如果是官方的东西，直接使用official  如果不是官方的东西，就物品代码后面加上.tex</t>
   </si>
   <si>
+    <t>是否常驻。常驻则填 yes</t>
+  </si>
+  <si>
     <t>木头</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t>log.tex</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>石头</t>
@@ -758,7 +764,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -768,8 +774,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1085,10 +1097,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1101,53 +1113,57 @@
     <col min="8" max="8" width="24.225" style="2" customWidth="1"/>
     <col min="9" max="9" width="26.95" style="2" customWidth="1"/>
     <col min="10" max="10" width="19.3666666666667" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="11" max="11" width="9" style="3"/>
+    <col min="12" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="76" customHeight="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="1" customFormat="1" ht="76" customHeight="1" spans="1:11">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -1159,27 +1175,30 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -1191,27 +1210,27 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -1223,27 +1242,27 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -1255,27 +1274,27 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -1287,27 +1306,27 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -1319,27 +1338,27 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -1351,27 +1370,27 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
@@ -1383,27 +1402,27 @@
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1415,27 +1434,27 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1447,27 +1466,27 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -1479,27 +1498,27 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
@@ -1511,13 +1530,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shop_sys_tool bug fix and new excample
</commit_message>
<xml_diff>
--- a/shop_sys_tool/shop_items_list.xlsx
+++ b/shop_sys_tool/shop_items_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
   <si>
     <t>物品</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>petals_evil</t>
+  </si>
+  <si>
+    <t>阿拜多斯高纯度合金</t>
+  </si>
+  <si>
+    <t>hoshino_item_abydos_high_purity_alloy</t>
+  </si>
+  <si>
+    <t>images/inventoryimages/hoshino_item_abydos_high_purity_alloy.xml</t>
+  </si>
+  <si>
+    <t>hoshino_item_abydos_high_purity_alloy.tex</t>
   </si>
 </sst>
 </file>
@@ -764,7 +776,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -774,14 +786,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1097,58 +1103,58 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="16.175" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.9666666666667" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.3333333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.5916666666667" style="2" customWidth="1"/>
     <col min="4" max="6" width="22.8083333333333" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2"/>
     <col min="8" max="8" width="24.225" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.95" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.3666666666667" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9" style="3"/>
-    <col min="12" max="16384" width="9" style="4"/>
+    <col min="9" max="9" width="67.8083333333333" style="2" customWidth="1"/>
+    <col min="10" max="10" width="47.575" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9" style="2"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="76" customHeight="1" spans="1:11">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1183,7 +1189,7 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1537,6 +1543,38 @@
       </c>
       <c r="J13" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24shop mouse over name colour change
</commit_message>
<xml_diff>
--- a/shop_sys_tool/shop_items_list.xlsx
+++ b/shop_sys_tool/shop_items_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
   <si>
     <t>物品</t>
   </si>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1545,7 +1545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -1568,13 +1568,16 @@
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>